<commit_message>
quick and dirty create jar with dependancies
</commit_message>
<xml_diff>
--- a/rule_processor_parent/workspace/kriterien.xlsx
+++ b/rule_processor_parent/workspace/kriterien.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekte\rule_editor\rule_editor\rule_processor_parent\workspace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED9A3272-F310-4A8E-812A-D360E2F2040D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54D811F3-F6DC-4771-998A-13D6BC5B571B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="5" activeTab="9" xr2:uid="{40394FAC-CA3C-4E1F-A8B2-430580AB5DA3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="3" xr2:uid="{40394FAC-CA3C-4E1F-A8B2-430580AB5DA3}"/>
   </bookViews>
   <sheets>
     <sheet name="Patient" sheetId="1" r:id="rId1"/>
@@ -1125,7 +1125,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80C18EC0-4CB4-40EB-AE9F-00F2A9F281EC}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -5647,8 +5647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFDEF641-09A1-4E83-A7F0-4D74D9CBFE96}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5763,6 +5763,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>